<commit_message>
Updated with tutor's feedback
</commit_message>
<xml_diff>
--- a/BurndownChart.xlsx
+++ b/BurndownChart.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\2017 sem 2\IFB299\assignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,8 +38,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,65 +201,142 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="20"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$29</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$B$29</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>3</c:v>
@@ -295,12 +380,89 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="20"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$29</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$2:$C$29</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42</c:v>
                 </c:pt>
@@ -320,7 +482,7 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>38</c:v>
@@ -347,13 +509,19 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,7 +573,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Timelne</a:t>
+                  <a:t>Timeline</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-AU" baseline="0"/>
@@ -444,6 +612,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1238,15 +1407,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1570,242 +1739,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>42</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1">
         <v>41</v>
       </c>
-      <c r="C3">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-      <c r="C4">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>39</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>38</v>
-      </c>
-      <c r="C6">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>37</v>
-      </c>
-      <c r="C7">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>35</v>
-      </c>
-      <c r="C8">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>31</v>
-      </c>
-      <c r="C9">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="C20" s="1">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>29</v>
-      </c>
-      <c r="C11">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>24</v>
-      </c>
-      <c r="C13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>